<commit_message>
insersion y exportacion de productos
</commit_message>
<xml_diff>
--- a/public/uploads/import/services.xlsx
+++ b/public/uploads/import/services.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel Mayansource\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ejemplo\public\uploads\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9C24CE-7EDA-445D-90DC-44C0A95D78CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="9720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -48,54 +49,46 @@
     <t>El nombre del proveedor debe ser exactamente el mismo registrado en el sistema.</t>
   </si>
   <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>PROVEEDOR</t>
-  </si>
-  <si>
-    <t>PUNTOS</t>
-  </si>
-  <si>
-    <t>COSTO</t>
-  </si>
-  <si>
-    <t>PRECIO ATENUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRECIO EMPRESAS </t>
-  </si>
-  <si>
-    <t>PRECIO SEGUROS</t>
-  </si>
-  <si>
     <t xml:space="preserve">FORMATO PARA IMPORTAR SERVICIOS </t>
   </si>
   <si>
-    <t>SUBCATEBORÍAS</t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>id_categoria</t>
+  </si>
+  <si>
+    <t>fotografia</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>id_proveedor</t>
+  </si>
+  <si>
+    <t>estado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -114,16 +107,18 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,19 +143,19 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,14 +435,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -456,87 +451,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>